<commit_message>
Finished Combined PCB and Gerber files
Combined pcb fits on 10x10cm, breakable and gerbers are finished for elecrow order. will order everything this weekend, lets see if it works.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25950" windowHeight="7815" tabRatio="839" activeTab="5"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25950" windowHeight="7815" tabRatio="967" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25950" windowHeight="7815" tabRatio="666" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Stepper Module" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,10 @@
     <sheet name="Heatbed Module" sheetId="5" r:id="rId4"/>
     <sheet name="Additional IRLML2502 Module" sheetId="6" r:id="rId5"/>
     <sheet name="Mainboard" sheetId="3" r:id="rId6"/>
-    <sheet name="Stock" sheetId="7" r:id="rId7"/>
-    <sheet name="Order List" sheetId="8" r:id="rId8"/>
-    <sheet name="Pers. Shopping List" sheetId="9" r:id="rId9"/>
+    <sheet name="Order List" sheetId="8" r:id="rId7"/>
+    <sheet name="Pers. Shopping List" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="214">
   <si>
     <t>Number</t>
   </si>
@@ -609,63 +607,6 @@
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Package</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
-    <t>Bin</t>
-  </si>
-  <si>
-    <t>Capacitor</t>
-  </si>
-  <si>
-    <t>0805</t>
-  </si>
-  <si>
-    <t>100nF, 50V</t>
-  </si>
-  <si>
-    <t>A1-A2</t>
-  </si>
-  <si>
-    <t>10nF</t>
-  </si>
-  <si>
-    <t>10uF, 16V</t>
-  </si>
-  <si>
-    <t>B1-B2</t>
-  </si>
-  <si>
-    <t>Resistor</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>B5-B6</t>
-  </si>
-  <si>
-    <t>100K</t>
-  </si>
-  <si>
-    <t>A4-A5</t>
-  </si>
-  <si>
-    <t>30pF</t>
-  </si>
-  <si>
     <t>Male Pinheader Straight 2.54mm 1x90</t>
   </si>
   <si>
@@ -694,6 +635,45 @@
   </si>
   <si>
     <t>http://goo.gl/SWVCW9</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>Order Quantity</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>SD*5</t>
+  </si>
+  <si>
+    <t>Price x Quan.</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>oder x5</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>http://goo.gl/Uk5B9L</t>
+  </si>
+  <si>
+    <t>Female Pinheader Angled 2.54mm 2x40</t>
+  </si>
+  <si>
+    <t>Platinen</t>
+  </si>
+  <si>
+    <t>1*10</t>
+  </si>
+  <si>
+    <t>BESTELLUNG TOTAL</t>
   </si>
 </sst>
 </file>
@@ -717,7 +697,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -748,6 +728,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -762,7 +748,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -771,12 +757,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1061,7 +1050,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -1101,13 +1090,13 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="7">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D2">
@@ -1296,7 +1285,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1305,7 +1294,7 @@
       </c>
       <c r="E11" s="1">
         <f>SUM(E2:E9)</f>
-        <v>2.3600000000000003</v>
+        <v>1.9600000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -1327,7 +1316,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -1418,13 +1407,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D4">
@@ -1470,13 +1459,13 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D6">
@@ -1535,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1544,7 +1533,7 @@
       </c>
       <c r="E10" s="1">
         <f>SUM(E2:E8)</f>
-        <v>1.3800000000000001</v>
+        <v>0.98</v>
       </c>
     </row>
   </sheetData>
@@ -1564,12 +1553,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1736,13 +1723,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D7">
@@ -1814,13 +1801,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D10">
@@ -1931,7 +1918,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -1941,7 +1928,7 @@
       </c>
       <c r="E16" s="1">
         <f>SUM(E2:E14)</f>
-        <v>2.2800000000000002</v>
+        <v>1.88</v>
       </c>
     </row>
   </sheetData>
@@ -1968,11 +1955,9 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:I15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2139,13 +2124,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D7">
@@ -2217,13 +2202,13 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D10">
@@ -2386,7 +2371,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
@@ -2395,7 +2380,7 @@
       </c>
       <c r="E18" s="1">
         <f>SUM(E2:E16)</f>
-        <v>2.74</v>
+        <v>2.3400000000000003</v>
       </c>
     </row>
   </sheetData>
@@ -2424,11 +2409,9 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A4:C4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A2" sqref="A2:I7"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2517,13 +2500,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D4">
@@ -2634,7 +2617,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>1</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2643,7 +2626,7 @@
       </c>
       <c r="E10" s="1">
         <f>SUM(E2:E8)</f>
-        <v>2.09</v>
+        <v>1.69</v>
       </c>
     </row>
   </sheetData>
@@ -2663,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -2720,7 +2703,7 @@
         <v>3.53</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="H2">
         <v>10</v>
@@ -3068,13 +3051,13 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="7">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D16">
@@ -3172,13 +3155,13 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D20">
@@ -3224,13 +3207,13 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>45</v>
       </c>
       <c r="D22">
@@ -3250,13 +3233,13 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>129</v>
       </c>
       <c r="D23">
@@ -3276,13 +3259,13 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>132</v>
       </c>
       <c r="D24">
@@ -3302,13 +3285,13 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>73</v>
       </c>
       <c r="D25">
@@ -3861,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -3870,7 +3853,7 @@
       </c>
       <c r="E48" s="1">
         <f>SUM(E2:E46)</f>
-        <v>14.409999999999997</v>
+        <v>15.409999999999997</v>
       </c>
     </row>
   </sheetData>
@@ -3925,175 +3908,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43:H46"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>100</v>
-      </c>
-      <c r="B2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" t="s">
-        <v>201</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>200</v>
-      </c>
-      <c r="B3" t="s">
-        <v>197</v>
-      </c>
-      <c r="C3" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>120</v>
-      </c>
-      <c r="B4" t="s">
-        <v>197</v>
-      </c>
-      <c r="C4" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>100</v>
-      </c>
-      <c r="B8" t="s">
-        <v>204</v>
-      </c>
-      <c r="C8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>100</v>
-      </c>
-      <c r="B9" t="s">
-        <v>204</v>
-      </c>
-      <c r="C9" t="s">
-        <v>207</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="E9">
-        <v>4</v>
-      </c>
-      <c r="F9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H2" sqref="F2:H2"/>
-    </sheetView>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="1">
-      <selection activeCell="L44" sqref="L44"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4142,7 +3963,7 @@
         <v>3.53</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -4406,42 +4227,42 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>175</v>
+        <v>119</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="G14">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H14">
-        <v>2.69</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>119</v>
+      <c r="A15" s="7">
+        <v>15</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15">
-        <v>0.04</v>
+        <v>0.02</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>177</v>
+        <v>49</v>
       </c>
       <c r="G15">
         <v>200</v>
@@ -4451,20 +4272,20 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>15</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>43</v>
+      <c r="A16" s="5">
+        <v>16</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>49</v>
+        <v>178</v>
       </c>
       <c r="G16">
         <v>200</v>
@@ -4475,19 +4296,19 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>68</v>
+        <v>123</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>0.03</v>
+        <v>0.01</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G17">
         <v>200</v>
@@ -4498,10 +4319,10 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -4510,7 +4331,7 @@
         <v>0.01</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G18">
         <v>200</v>
@@ -4520,20 +4341,20 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>124</v>
+      <c r="A19" s="7">
+        <v>19</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D19">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>180</v>
+        <v>95</v>
       </c>
       <c r="G19">
         <v>200</v>
@@ -4543,20 +4364,20 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>19</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>9</v>
+      <c r="A20" s="5">
+        <v>20</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="C20">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D20">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G20">
         <v>200</v>
@@ -4566,43 +4387,43 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>126</v>
+      <c r="A21" s="7">
+        <v>21</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D21">
-        <v>0.01</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="G21">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="H21">
-        <v>0.55000000000000004</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
-        <v>21</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>45</v>
+      <c r="A22" s="7">
+        <v>22</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="C22">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D22">
-        <v>7.0000000000000007E-2</v>
+        <v>0.05</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>51</v>
+        <v>165</v>
       </c>
       <c r="G22">
         <v>100</v>
@@ -4612,688 +4433,2079 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
-        <v>22</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>129</v>
+      <c r="A23" s="7">
+        <v>23</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="C23">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D23">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G23">
         <v>100</v>
       </c>
       <c r="H23">
-        <v>0.7</v>
+        <v>0.72</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="8">
-        <v>23</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>132</v>
+      <c r="A24" s="7">
+        <v>24</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="C24">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>164</v>
+        <v>74</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H24">
-        <v>0.72</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="8">
-        <v>24</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>73</v>
+      <c r="A25" s="5">
+        <v>25</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="C25">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <v>0.1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>74</v>
+        <v>163</v>
       </c>
       <c r="G25">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="H25">
-        <v>0.92</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G26">
         <v>20</v>
       </c>
       <c r="H26">
-        <v>1.81</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="G27">
         <v>20</v>
       </c>
       <c r="H27">
-        <v>1.72</v>
+        <v>1.81</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D28">
-        <v>0.1</v>
+        <v>0.75</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>162</v>
+        <v>12</v>
       </c>
       <c r="G28">
         <v>20</v>
       </c>
       <c r="H28">
-        <v>1.81</v>
+        <v>2.42</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>160</v>
+        <v>22</v>
       </c>
       <c r="C29">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D29">
-        <v>0.75</v>
+        <v>0.42</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H29">
-        <v>2.42</v>
+        <v>3.34</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>22</v>
+        <v>191</v>
       </c>
       <c r="C30">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D30">
-        <v>0.42</v>
+        <v>0.15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30">
-        <v>100</v>
+        <v>14</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H30">
-        <v>3.34</v>
+        <v>0.61</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>0.15</v>
+        <v>0.45</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H31">
-        <v>0.61</v>
+        <v>0.89</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>212</v>
+        <v>155</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32">
-        <v>0.45</v>
+        <v>1.41</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>24</v>
+        <v>154</v>
+      </c>
+      <c r="G32">
+        <v>10</v>
       </c>
       <c r="H32">
-        <v>0.89</v>
+        <v>4.63</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>155</v>
+        <v>27</v>
       </c>
       <c r="C33">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D33">
-        <v>1.41</v>
+        <v>2.72</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>154</v>
+        <v>28</v>
       </c>
       <c r="G33">
         <v>10</v>
       </c>
       <c r="H33">
-        <v>4.63</v>
+        <v>3.33</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
       <c r="C34">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>2.72</v>
+        <v>0.33</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H34">
-        <v>3.33</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C35">
         <v>2</v>
       </c>
       <c r="D35">
-        <v>0.33</v>
+        <v>0.5</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G35">
         <v>20</v>
       </c>
       <c r="H35">
-        <v>3.04</v>
+        <v>4.6399999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
-        <v>44</v>
+        <v>1</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="G36">
         <v>20</v>
       </c>
       <c r="H36">
-        <v>4.6399999999999997</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C37">
         <v>3</v>
       </c>
       <c r="D37">
-        <v>0.45</v>
+        <v>1.6</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>64</v>
+        <v>209</v>
       </c>
       <c r="G37">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="H37">
-        <v>2.8</v>
+        <v>25.87</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="C38">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D38">
-        <v>1.6</v>
+        <v>0.1</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="G38">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="H38">
-        <v>10.56</v>
+        <v>1.24</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
+        <v>4</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39">
         <v>3</v>
       </c>
-      <c r="B39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39">
-        <v>4</v>
-      </c>
       <c r="D39">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="G39">
         <v>100</v>
       </c>
       <c r="H39">
-        <v>1.24</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
+        <v>8</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
         <v>4</v>
       </c>
-      <c r="B40" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="C40">
-        <v>3</v>
-      </c>
       <c r="D40">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="G40">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H40">
-        <v>1.21</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>44</v>
+        <v>192</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <v>0.02</v>
+        <v>0.75</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G41">
-        <v>200</v>
+        <v>48</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="H41">
-        <v>0.55000000000000004</v>
+        <v>3.43</v>
+      </c>
+      <c r="K41">
+        <f>SUM(D2:D47)</f>
+        <v>23.38</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>211</v>
+        <v>77</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D42">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>24</v>
+        <v>80</v>
+      </c>
+      <c r="G42">
+        <v>20</v>
       </c>
       <c r="H42">
-        <v>3.43</v>
-      </c>
-      <c r="K42">
-        <f>SUM(D2:D48)</f>
-        <v>23.41</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D43">
-        <v>0.6</v>
+        <v>0.26</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="G43">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="H43">
-        <v>3.7</v>
+        <v>2.59</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C44">
         <v>1</v>
       </c>
       <c r="D44">
-        <v>0.26</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="G44">
         <v>10</v>
       </c>
       <c r="H44">
-        <v>2.59</v>
+        <v>0.59</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>7.0000000000000007E-2</v>
+        <v>0.2</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>52</v>
+        <v>93</v>
       </c>
       <c r="G45">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="H45">
-        <v>0.59</v>
+        <v>4.76</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G46">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="H46">
-        <v>4.76</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="5">
-        <v>2</v>
+      <c r="A47" s="8" t="s">
+        <v>29</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>90</v>
+        <v>194</v>
       </c>
       <c r="C47">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D47">
-        <v>0.02</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47">
-        <v>200</v>
-      </c>
-      <c r="H47">
-        <v>0.55000000000000004</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C48">
-        <v>6</v>
-      </c>
-      <c r="D48">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F30" r:id="rId1"/>
-    <hyperlink ref="F29" r:id="rId2"/>
-    <hyperlink ref="F32" r:id="rId3"/>
-    <hyperlink ref="F31" r:id="rId4"/>
-    <hyperlink ref="F36" r:id="rId5"/>
-    <hyperlink ref="F20" r:id="rId6"/>
-    <hyperlink ref="F21" r:id="rId7"/>
-    <hyperlink ref="F16" r:id="rId8"/>
-    <hyperlink ref="F22" r:id="rId9"/>
-    <hyperlink ref="F25" r:id="rId10"/>
-    <hyperlink ref="F35" r:id="rId11"/>
-    <hyperlink ref="F34" r:id="rId12"/>
-    <hyperlink ref="F33" r:id="rId13"/>
+    <hyperlink ref="F29" r:id="rId1"/>
+    <hyperlink ref="F28" r:id="rId2"/>
+    <hyperlink ref="F31" r:id="rId3"/>
+    <hyperlink ref="F30" r:id="rId4"/>
+    <hyperlink ref="F35" r:id="rId5"/>
+    <hyperlink ref="F19" r:id="rId6"/>
+    <hyperlink ref="F20" r:id="rId7"/>
+    <hyperlink ref="F15" r:id="rId8"/>
+    <hyperlink ref="F21" r:id="rId9"/>
+    <hyperlink ref="F24" r:id="rId10"/>
+    <hyperlink ref="F34" r:id="rId11"/>
+    <hyperlink ref="F33" r:id="rId12"/>
+    <hyperlink ref="F32" r:id="rId13"/>
     <hyperlink ref="F9" r:id="rId14"/>
-    <hyperlink ref="F27" r:id="rId15"/>
-    <hyperlink ref="F28" r:id="rId16"/>
-    <hyperlink ref="F26" r:id="rId17"/>
-    <hyperlink ref="F24" r:id="rId18"/>
-    <hyperlink ref="F23" r:id="rId19"/>
+    <hyperlink ref="F26" r:id="rId15"/>
+    <hyperlink ref="F27" r:id="rId16"/>
+    <hyperlink ref="F25" r:id="rId17"/>
+    <hyperlink ref="F23" r:id="rId18"/>
+    <hyperlink ref="F22" r:id="rId19"/>
     <hyperlink ref="F11" r:id="rId20"/>
     <hyperlink ref="F13" r:id="rId21"/>
     <hyperlink ref="F14" r:id="rId22"/>
-    <hyperlink ref="F15" r:id="rId23"/>
+    <hyperlink ref="F16" r:id="rId23"/>
     <hyperlink ref="F17" r:id="rId24"/>
     <hyperlink ref="F18" r:id="rId25"/>
-    <hyperlink ref="F19" r:id="rId26"/>
-    <hyperlink ref="F10" r:id="rId27"/>
-    <hyperlink ref="F12" r:id="rId28"/>
-    <hyperlink ref="F7" r:id="rId29"/>
-    <hyperlink ref="F4" r:id="rId30"/>
-    <hyperlink ref="F3" r:id="rId31"/>
-    <hyperlink ref="F8" r:id="rId32"/>
-    <hyperlink ref="F5" r:id="rId33"/>
-    <hyperlink ref="F6" r:id="rId34"/>
-    <hyperlink ref="F37" r:id="rId35"/>
-    <hyperlink ref="F38" r:id="rId36"/>
-    <hyperlink ref="F39" r:id="rId37"/>
-    <hyperlink ref="F40" r:id="rId38"/>
-    <hyperlink ref="F41" r:id="rId39"/>
-    <hyperlink ref="F42" r:id="rId40"/>
-    <hyperlink ref="F43" r:id="rId41"/>
-    <hyperlink ref="F45" r:id="rId42"/>
-    <hyperlink ref="F46" r:id="rId43"/>
-    <hyperlink ref="F47" r:id="rId44"/>
-    <hyperlink ref="F44" r:id="rId45"/>
+    <hyperlink ref="F10" r:id="rId26"/>
+    <hyperlink ref="F12" r:id="rId27"/>
+    <hyperlink ref="F7" r:id="rId28"/>
+    <hyperlink ref="F4" r:id="rId29"/>
+    <hyperlink ref="F3" r:id="rId30"/>
+    <hyperlink ref="F8" r:id="rId31"/>
+    <hyperlink ref="F5" r:id="rId32"/>
+    <hyperlink ref="F6" r:id="rId33"/>
+    <hyperlink ref="F36" r:id="rId34"/>
+    <hyperlink ref="F38" r:id="rId35"/>
+    <hyperlink ref="F39" r:id="rId36"/>
+    <hyperlink ref="F40" r:id="rId37"/>
+    <hyperlink ref="F41" r:id="rId38"/>
+    <hyperlink ref="F42" r:id="rId39"/>
+    <hyperlink ref="F44" r:id="rId40"/>
+    <hyperlink ref="F45" r:id="rId41"/>
+    <hyperlink ref="F46" r:id="rId42"/>
+    <hyperlink ref="F43" r:id="rId43"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="1">
+      <selection activeCell="D51" sqref="D51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" customWidth="1"/>
-    <col min="4" max="4" width="32" customWidth="1"/>
-    <col min="5" max="5" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>214</v>
+        <v>195</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>196</v>
       </c>
       <c r="C1" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="E1" t="s">
-        <v>218</v>
+        <v>199</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>34.32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E6">
+        <v>30</v>
+      </c>
+      <c r="F6">
+        <v>9.3699999999999992</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>8.5399999999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E8">
+        <v>60</v>
+      </c>
+      <c r="F8">
+        <v>1.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>2.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>3.3</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>1.85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>3.92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E16">
+        <v>200</v>
+      </c>
+      <c r="F16">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17">
+        <v>200</v>
+      </c>
+      <c r="F17">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18">
+        <v>45</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E18">
+        <v>200</v>
+      </c>
+      <c r="F18">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E19">
+        <v>200</v>
+      </c>
+      <c r="F19">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20">
+        <v>200</v>
+      </c>
+      <c r="F20">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>80</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21">
+        <v>200</v>
+      </c>
+      <c r="F21">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22">
+        <v>200</v>
+      </c>
+      <c r="F22">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23">
+        <v>85</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>1.4</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24">
+        <v>60</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>0.7</v>
+      </c>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>0.72</v>
+      </c>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26">
+        <v>35</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E26">
+        <v>50</v>
+      </c>
+      <c r="F26">
+        <v>1.84</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>1.81</v>
+      </c>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>3.44</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>26</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>1.81</v>
+      </c>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>27</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C30">
+        <v>50</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>7.26</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>28</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31">
+        <v>100</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <v>6.68</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32">
+        <v>1.83</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>30</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33">
+        <v>3.56</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="H33" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>31</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C34">
+        <v>30</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34">
+        <v>13.89</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>32</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35">
+        <v>10</v>
+      </c>
+      <c r="F35">
+        <v>19.98</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>33</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C36">
+        <v>20</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>3.04</v>
+      </c>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>34</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37">
+        <v>20</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>35</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>5.6</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>36</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>25</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E39">
+        <v>50</v>
+      </c>
+      <c r="F39">
+        <v>25.87</v>
+      </c>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>37</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>30</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40">
+        <v>100</v>
+      </c>
+      <c r="F40">
+        <v>1.24</v>
+      </c>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>38</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C41">
+        <v>25</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E41">
+        <v>100</v>
+      </c>
+      <c r="F41">
+        <v>1.21</v>
+      </c>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>39</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42">
+        <v>30</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42">
+        <v>200</v>
+      </c>
+      <c r="F42">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>40</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43">
+        <v>3.43</v>
+      </c>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>41</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44">
+        <v>25</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <v>7.4</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>42</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C45">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E45">
+        <v>10</v>
+      </c>
+      <c r="F45">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>43</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>44</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C47">
+        <v>20</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E47">
+        <v>100</v>
+      </c>
+      <c r="F47">
+        <v>4.76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>45</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C48">
+        <v>20</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E48">
+        <v>200</v>
+      </c>
+      <c r="F48">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>46</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F49">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>48</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E51" s="9"/>
+      <c r="F51" s="10">
+        <f>SUM(F4:F49)</f>
+        <v>268.33000000000004</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D51:E51"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1"/>
+    <hyperlink ref="D13" r:id="rId2"/>
+    <hyperlink ref="D15" r:id="rId3"/>
+    <hyperlink ref="D16" r:id="rId4"/>
+    <hyperlink ref="D12" r:id="rId5"/>
+    <hyperlink ref="D14" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D6" r:id="rId8"/>
+    <hyperlink ref="D5" r:id="rId9"/>
+    <hyperlink ref="D10" r:id="rId10"/>
+    <hyperlink ref="D7" r:id="rId11"/>
+    <hyperlink ref="D8" r:id="rId12"/>
+    <hyperlink ref="D17" r:id="rId13"/>
+    <hyperlink ref="D19" r:id="rId14"/>
+    <hyperlink ref="D20" r:id="rId15"/>
+    <hyperlink ref="D18" r:id="rId16"/>
+    <hyperlink ref="D21" r:id="rId17"/>
+    <hyperlink ref="D22" r:id="rId18"/>
+    <hyperlink ref="D23" r:id="rId19"/>
+    <hyperlink ref="D26" r:id="rId20"/>
+    <hyperlink ref="D25" r:id="rId21"/>
+    <hyperlink ref="D24" r:id="rId22"/>
+    <hyperlink ref="D30" r:id="rId23"/>
+    <hyperlink ref="D28" r:id="rId24"/>
+    <hyperlink ref="D29" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D31" r:id="rId27"/>
+    <hyperlink ref="D33" r:id="rId28"/>
+    <hyperlink ref="D32" r:id="rId29"/>
+    <hyperlink ref="D36" r:id="rId30"/>
+    <hyperlink ref="D35" r:id="rId31"/>
+    <hyperlink ref="D34" r:id="rId32"/>
+    <hyperlink ref="D37" r:id="rId33"/>
+    <hyperlink ref="D38" r:id="rId34"/>
+    <hyperlink ref="D40" r:id="rId35"/>
+    <hyperlink ref="D41" r:id="rId36"/>
+    <hyperlink ref="D42" r:id="rId37"/>
+    <hyperlink ref="D43" r:id="rId38"/>
+    <hyperlink ref="D44" r:id="rId39"/>
+    <hyperlink ref="D46" r:id="rId40"/>
+    <hyperlink ref="D47" r:id="rId41"/>
+    <hyperlink ref="D48" r:id="rId42"/>
+    <hyperlink ref="D45" r:id="rId43"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Reworked Modules to sit ontop of the mainboard
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,8 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25950" windowHeight="7815" tabRatio="666" firstSheet="4" activeTab="6"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25950" windowHeight="7815" tabRatio="666" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Stepper Module" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,9 @@
     <sheet name="Additional IRLML2502 Module" sheetId="6" r:id="rId5"/>
     <sheet name="Mainboard" sheetId="3" r:id="rId6"/>
     <sheet name="Order List" sheetId="8" r:id="rId7"/>
-    <sheet name="Pers. Shopping List" sheetId="9" r:id="rId8"/>
+    <sheet name="Tabelle1" sheetId="10" r:id="rId8"/>
+    <sheet name="Pers. Shopping List" sheetId="9" r:id="rId9"/>
+    <sheet name="New Thing V2" sheetId="11" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="216">
   <si>
     <t>Number</t>
   </si>
@@ -674,6 +675,12 @@
   </si>
   <si>
     <t>BESTELLUNG TOTAL</t>
+  </si>
+  <si>
+    <t>Fuse holder</t>
+  </si>
+  <si>
+    <t>http://de.farnell.com/keystone/3544/fuse-holder-0-8-x-2-8mm-pcb-mount/dp/2301268</t>
   </si>
 </sst>
 </file>
@@ -697,7 +704,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,6 +741,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -748,7 +761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -762,10 +775,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -785,9 +799,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -825,7 +839,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -897,7 +911,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1052,7 +1066,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1311,6 +1324,29 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I10"/>
@@ -1318,7 +1354,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1556,7 +1591,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1957,7 +1991,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2411,7 +2444,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2646,10 +2678,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3910,11 +3941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43:H46"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3950,10 +3978,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>103</v>
       </c>
       <c r="C2">
@@ -3973,10 +4001,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="10" t="s">
         <v>104</v>
       </c>
       <c r="C3">
@@ -3996,10 +4024,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="10" t="s">
         <v>105</v>
       </c>
       <c r="C4">
@@ -4019,10 +4047,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="10" t="s">
         <v>106</v>
       </c>
       <c r="C5">
@@ -4042,10 +4070,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>108</v>
       </c>
       <c r="C6">
@@ -4065,10 +4093,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>183</v>
       </c>
       <c r="C7">
@@ -4088,10 +4116,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="10" t="s">
         <v>138</v>
       </c>
       <c r="C8">
@@ -4111,10 +4139,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>115</v>
       </c>
       <c r="C9">
@@ -4134,10 +4162,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="10" t="s">
         <v>117</v>
       </c>
       <c r="C10">
@@ -4157,10 +4185,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="10" t="s">
         <v>170</v>
       </c>
       <c r="C11">
@@ -4180,10 +4208,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="10" t="s">
         <v>113</v>
       </c>
       <c r="C12">
@@ -4203,10 +4231,10 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="10" t="s">
         <v>172</v>
       </c>
       <c r="C13">
@@ -4226,10 +4254,10 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="10">
         <v>14</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="10" t="s">
         <v>119</v>
       </c>
       <c r="C14">
@@ -4249,10 +4277,10 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
+      <c r="A15" s="10">
         <v>15</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="10" t="s">
         <v>43</v>
       </c>
       <c r="C15">
@@ -4272,10 +4300,10 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="10">
         <v>16</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C16">
@@ -4295,10 +4323,10 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="10">
         <v>17</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C17">
@@ -4318,10 +4346,10 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="10">
         <v>18</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="10" t="s">
         <v>124</v>
       </c>
       <c r="C18">
@@ -4341,10 +4369,10 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
+      <c r="A19" s="10">
         <v>19</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C19">
@@ -4364,10 +4392,10 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+      <c r="A20" s="10">
         <v>20</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="10" t="s">
         <v>126</v>
       </c>
       <c r="C20">
@@ -4387,10 +4415,10 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+      <c r="A21" s="10">
         <v>21</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="10" t="s">
         <v>45</v>
       </c>
       <c r="C21">
@@ -4410,10 +4438,10 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+      <c r="A22" s="10">
         <v>22</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="10" t="s">
         <v>129</v>
       </c>
       <c r="C22">
@@ -4433,10 +4461,10 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
+      <c r="A23" s="10">
         <v>23</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="10" t="s">
         <v>132</v>
       </c>
       <c r="C23">
@@ -4456,10 +4484,10 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="10">
         <v>24</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="10" t="s">
         <v>73</v>
       </c>
       <c r="C24">
@@ -4479,10 +4507,10 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="10">
         <v>25</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="10" t="s">
         <v>159</v>
       </c>
       <c r="C25">
@@ -4502,10 +4530,10 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="5">
+      <c r="A26" s="10">
         <v>26</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="10" t="s">
         <v>157</v>
       </c>
       <c r="C26">
@@ -4525,10 +4553,10 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+      <c r="A27" s="10">
         <v>27</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="10" t="s">
         <v>158</v>
       </c>
       <c r="C27">
@@ -4548,10 +4576,10 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
+      <c r="A28" s="10">
         <v>28</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="10" t="s">
         <v>160</v>
       </c>
       <c r="C28">
@@ -4571,10 +4599,10 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
+      <c r="A29" s="10">
         <v>29</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C29">
@@ -4594,10 +4622,10 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
+      <c r="A30" s="10">
         <v>30</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="10" t="s">
         <v>191</v>
       </c>
       <c r="C30">
@@ -4617,10 +4645,10 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
+      <c r="A31" s="10">
         <v>34</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="10" t="s">
         <v>193</v>
       </c>
       <c r="C31">
@@ -4640,10 +4668,10 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+      <c r="A32" s="10">
         <v>41</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="10" t="s">
         <v>155</v>
       </c>
       <c r="C32">
@@ -4663,10 +4691,10 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
+      <c r="A33" s="10">
         <v>42</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C33">
@@ -4686,10 +4714,10 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="10">
         <v>43</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="10" t="s">
         <v>78</v>
       </c>
       <c r="C34">
@@ -4709,10 +4737,10 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
+      <c r="A35" s="10">
         <v>44</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="10" t="s">
         <v>83</v>
       </c>
       <c r="C35">
@@ -4732,10 +4760,10 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>1</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="10">
+        <v>1</v>
+      </c>
+      <c r="B36" s="10" t="s">
         <v>63</v>
       </c>
       <c r="C36">
@@ -4755,10 +4783,10 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+      <c r="A37" s="10">
         <v>2</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="10" t="s">
         <v>65</v>
       </c>
       <c r="C37">
@@ -4778,10 +4806,10 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="10">
         <v>3</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="10" t="s">
         <v>41</v>
       </c>
       <c r="C38">
@@ -4801,10 +4829,10 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="10">
         <v>4</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="10" t="s">
         <v>114</v>
       </c>
       <c r="C39">
@@ -4824,10 +4852,10 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="10">
         <v>8</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C40">
@@ -4847,10 +4875,10 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="10">
         <v>11</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="10" t="s">
         <v>192</v>
       </c>
       <c r="C41">
@@ -4874,10 +4902,10 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="10">
         <v>12</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C42">
@@ -4897,10 +4925,10 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
-        <v>1</v>
-      </c>
-      <c r="B43" s="5" t="s">
+      <c r="A43" s="10">
+        <v>1</v>
+      </c>
+      <c r="B43" s="10" t="s">
         <v>39</v>
       </c>
       <c r="C43">
@@ -4920,10 +4948,10 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="5">
+      <c r="A44" s="10">
         <v>6</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="10" t="s">
         <v>46</v>
       </c>
       <c r="C44">
@@ -4943,10 +4971,10 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="5">
-        <v>1</v>
-      </c>
-      <c r="B45" s="5" t="s">
+      <c r="A45" s="10">
+        <v>1</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>89</v>
       </c>
       <c r="C45">
@@ -4966,10 +4994,10 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="5">
+      <c r="A46" s="10">
         <v>2</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="10" t="s">
         <v>90</v>
       </c>
       <c r="C46">
@@ -5047,6 +5075,7 @@
     <hyperlink ref="F45" r:id="rId41"/>
     <hyperlink ref="F46" r:id="rId42"/>
     <hyperlink ref="F43" r:id="rId43"/>
+    <hyperlink ref="F2" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5054,13 +5083,22 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E39" sqref="E39"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B21" workbookViewId="1">
-      <selection activeCell="D51" sqref="D51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6093,11 +6131,11 @@
       <c r="A51">
         <v>48</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="E51" s="9"/>
-      <c r="F51" s="10">
+      <c r="E51" s="11"/>
+      <c r="F51" s="9">
         <f>SUM(F4:F49)</f>
         <v>268.33000000000004</v>
       </c>

</xml_diff>